<commit_message>
Sorted list by chapter
</commit_message>
<xml_diff>
--- a/ScopeOfChapters.xlsx
+++ b/ScopeOfChapters.xlsx
@@ -331,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -365,6 +365,19 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -372,40 +385,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF333333"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color rgb="FFDDDDDD"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFDDDDDD"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -515,13 +494,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color rgb="FFDDDDDD"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color rgb="FFDDDDDD"/>
         </left>
@@ -531,6 +503,47 @@
         <top style="medium">
           <color rgb="FFDDDDDD"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color rgb="FFDDDDDD"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color rgb="FFDDDDDD"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFDDDDDD"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -547,13 +560,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D37" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D37" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A1:D37"/>
+  <sortState ref="A2:D37">
+    <sortCondition ref="D1:D37"/>
+  </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Topic" dataDxfId="4"/>
-    <tableColumn id="2" name="Sub-topic" dataDxfId="3"/>
-    <tableColumn id="3" name="Description" dataDxfId="2"/>
-    <tableColumn id="4" name="Chapter" dataDxfId="1"/>
+    <tableColumn id="1" name="Topic" dataDxfId="3"/>
+    <tableColumn id="2" name="Sub-topic" dataDxfId="2"/>
+    <tableColumn id="3" name="Description" dataDxfId="1"/>
+    <tableColumn id="4" name="Chapter" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -825,7 +841,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,88 +880,88 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D3" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="8">
-        <v>11</v>
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="7">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="8">
-        <v>13</v>
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="7">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -962,144 +978,144 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="8">
+    <row r="10" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="8">
+      <c r="C18" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="7">
+      <c r="D18" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>35</v>
+      <c r="B19" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>18</v>
       </c>
       <c r="D19" s="9">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1116,242 +1132,242 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D21" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D22" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="9">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D24" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D25" s="9">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="B27" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D27" s="9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D28" s="9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D29" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D30" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D35" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" s="9">
+      <c r="D32" s="17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" s="9">
-        <v>4</v>
+      <c r="C33" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="17">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>